<commit_message>
added 2nd semester courses link
</commit_message>
<xml_diff>
--- a/BCA(OL)_ASSIGNMENT.xlsx
+++ b/BCA(OL)_ASSIGNMENT.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishaan.kothidar\Documents\GitHub\BCAOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6129158\Projects\extras\BCAOL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7A125C-6CC9-4EB1-8E44-217153A7CBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AC36C0-CEBE-49F3-96C6-C6C7292CFC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{46359B33-B8D4-457A-8C07-85922C7B8647}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{46359B33-B8D4-457A-8C07-85922C7B8647}"/>
   </bookViews>
   <sheets>
     <sheet name="Semester1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Semester2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Semester1!$A$1:$A$17</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>Subjects</t>
   </si>
@@ -97,6 +98,36 @@
   </si>
   <si>
     <t>Seminar - 1</t>
+  </si>
+  <si>
+    <t>General Proficiency/NCC/Sports/Yoga/Seminar/</t>
+  </si>
+  <si>
+    <t>Object-Oriented Programming Laboratory</t>
+  </si>
+  <si>
+    <t>Data Structures Laboratory</t>
+  </si>
+  <si>
+    <t>Environmental Science</t>
+  </si>
+  <si>
+    <t>Indian Constitution</t>
+  </si>
+  <si>
+    <t>Indian Culture</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>Introduction to Operating Systems</t>
+  </si>
+  <si>
+    <t>Introduction to Object-Oriented Programming</t>
+  </si>
+  <si>
+    <t>Data Structures and File Organization</t>
   </si>
 </sst>
 </file>
@@ -478,20 +509,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC8AF22-169A-4F1A-80C8-A4113118EB96}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -508,7 +539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -522,7 +553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -539,7 +570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -556,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -584,7 +615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -601,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -618,7 +649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -635,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -649,31 +680,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="P16" s="4"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="16:17" x14ac:dyDescent="0.45">
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
@@ -718,6 +749,188 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79FA370-F25F-4907-9A9C-CC9BDBB953BA}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" tooltip="General Proficiency/NCC/Sports/Yoga/Seminar/Science of Happiness" display="https://lms.geuonline.com/d2l/home/7284" xr:uid="{35AF24BF-96CC-4FBB-BD22-BD3AD75FBB92}"/>
+    <hyperlink ref="A3" r:id="rId2" tooltip="Data Structures Laboratory" display="https://lms.geuonline.com/d2l/home/7276" xr:uid="{9A89056B-72A9-4109-87A3-E5FC9EC9943A}"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="Environmental Science" display="https://lms.geuonline.com/d2l/home/7283" xr:uid="{60F90554-A5B4-4547-8555-1EF4C4369A2E}"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="Object-Oriented Programming Laboratory" display="https://lms.geuonline.com/d2l/home/7277" xr:uid="{073CA52A-FA1D-4772-BD3E-23C67F44E056}"/>
+    <hyperlink ref="A6" r:id="rId5" tooltip="Indian Constitution" display="https://lms.geuonline.com/d2l/home/7279" xr:uid="{3605C8EB-7423-472E-8D6D-0E165E5C74FD}"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="Indian Culture" display="https://lms.geuonline.com/d2l/home/7280" xr:uid="{4386E46E-365F-497A-99E0-BD6265F57DD2}"/>
+    <hyperlink ref="A8" r:id="rId7" tooltip="Discrete Mathematics" display="https://lms.geuonline.com/d2l/home/7275" xr:uid="{8845BE5F-855B-4FE5-B4AC-246A339E9C82}"/>
+    <hyperlink ref="A9" r:id="rId8" tooltip="Introduction to Operating Systems" display="https://lms.geuonline.com/d2l/home/7274" xr:uid="{9F400D77-FDE6-4A87-ABC9-D8E1B9F2BFF5}"/>
+    <hyperlink ref="A10" r:id="rId9" tooltip="Introduction to Object-Oriented Programming" display="https://lms.geuonline.com/d2l/home/7281" xr:uid="{758AFB29-2A3B-42B0-9EF5-FA9BEFA0251F}"/>
+    <hyperlink ref="A11" r:id="rId10" tooltip="Data Structures and File Organization" display="https://lms.geuonline.com/d2l/home/7282" xr:uid="{43A6C3DF-9620-4830-A0CF-468468703AC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Entry" error="Select value from dropdown" xr:uid="{45A27309-C72D-4FC5-84B4-B8A95D617205}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Entry" error="Select values from dropdown" xr:uid="{D74D6EEB-58B4-4A7E-9BD8-441B9DECAA0B}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD1067B-2C9C-4B51-80DF-958DE6025D8C}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -725,32 +938,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>

</xml_diff>